<commit_message>
ajout de la carte conn batterie
</commit_message>
<xml_diff>
--- a/2-PROJ/18-Panel_2020/Project Outputs for Panel_2020/autre_BOM/BOM-Goldorak_RS.xlsx
+++ b/2-PROJ/18-Panel_2020/Project Outputs for Panel_2020/autre_BOM/BOM-Goldorak_RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\2-PROJ\18-Panel_2020\Project Outputs for Panel_2020\autre_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC183250-4D6E-4444-8CEA-9C1F01E8B991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7A4875-F20E-4A5A-8E75-09A75393512F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2535" windowWidth="29040" windowHeight="16440" xr2:uid="{408920D6-2028-46AB-B387-62A2998BA43A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{408920D6-2028-46AB-B387-62A2998BA43A}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM RS" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BOM RS'!$A$2:$G$15</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>BOM Goldorak 2020 - RS - via Evolutek</t>
   </si>
@@ -179,6 +179,27 @@
   </si>
   <si>
     <t>Montant</t>
+  </si>
+  <si>
+    <t>RS_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251-643 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pince coupante </t>
+  </si>
+  <si>
+    <t>Evo_1</t>
+  </si>
+  <si>
+    <t>contribution BBQ coupe</t>
+  </si>
+  <si>
+    <t>Evo_2</t>
+  </si>
+  <si>
+    <t>sweat Table ronde</t>
   </si>
 </sst>
 </file>
@@ -320,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -385,42 +406,39 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,11 +451,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,12 +768,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D818B09-7270-4533-8261-018D4E26A5CC}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,12 +789,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -827,7 +842,7 @@
         <f>E3</f>
         <v>5</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="33">
         <v>55.18</v>
       </c>
     </row>
@@ -851,7 +866,7 @@
         <f t="shared" ref="F4:F8" si="0">E4</f>
         <v>10</v>
       </c>
-      <c r="G4" s="35"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -873,7 +888,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G5" s="35"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -895,7 +910,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -917,7 +932,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
@@ -939,7 +954,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="36"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,7 +976,7 @@
       <c r="F9" s="1">
         <v>10</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="36">
         <v>279.98</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -987,7 +1002,7 @@
       <c r="F10" s="15">
         <v>28</v>
       </c>
-      <c r="G10" s="35"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1009,32 +1024,32 @@
       <c r="F11" s="20">
         <v>3</v>
       </c>
-      <c r="G11" s="36"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="22">
         <v>209</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <v>2</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <v>2</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="36">
         <v>77.86</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1055,7 +1070,7 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="35"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1073,7 +1088,7 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="G14" s="35"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1094,7 +1109,7 @@
       <c r="F15" s="1">
         <v>2</v>
       </c>
-      <c r="G15" s="35"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1112,7 +1127,7 @@
       <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="35"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1133,13 +1148,13 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G17" s="35"/>
+      <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>215</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="31" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1154,34 +1169,38 @@
       <c r="F18" s="15">
         <v>1</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
+      <c r="A19" s="22">
         <v>216</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="26">
         <v>2</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="23"/>
+      <c r="F19" s="26">
+        <v>2</v>
+      </c>
+      <c r="G19" s="36">
+        <v>28.97</v>
+      </c>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>217</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1193,16 +1212,19 @@
       <c r="E20" s="1">
         <v>1</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>218</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="29" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -1211,13 +1233,76 @@
       <c r="E21" s="15">
         <v>1</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="33"/>
+      <c r="F21" s="15">
+        <v>1</v>
+      </c>
+      <c r="G21" s="35"/>
       <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>219</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="36">
+        <f>(33.06/2)+4*3.6+37.3</f>
+        <v>68.22999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>220</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>221</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="37"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:G15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G22:G24"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G19:G21"/>
     <mergeCell ref="G3:G8"/>

</xml_diff>